<commit_message>
se realiza comentarios en el codigo
</commit_message>
<xml_diff>
--- a/parametrizacion.xlsx
+++ b/parametrizacion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\robot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Documents\Tita\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F5DB1A7-4E1F-4D82-B8A1-F11DA01C11D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FBE7F1-A5BF-4964-A345-5D8BBD2745DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{91D52C05-83E3-46A9-BAB2-AD1119661F3A}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{91D52C05-83E3-46A9-BAB2-AD1119661F3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -57,9 +57,6 @@
     <t>reportehorasGlobalDesing</t>
   </si>
   <si>
-    <t>camilotobon21@gmail.com</t>
-  </si>
-  <si>
     <t>correoArqDigit</t>
   </si>
   <si>
@@ -222,19 +219,19 @@
     <t>En el adjunto se encuentra el detalle de los empleados que tuvieron horas extras, quedan pendiente de aprobacion para pago.</t>
   </si>
   <si>
-    <t>C:/Desktop/Tita/</t>
-  </si>
-  <si>
-    <t>C:/Desktop/Tita/Docs/</t>
-  </si>
-  <si>
-    <t>Julio.Correal@ArqDigit.co</t>
-  </si>
-  <si>
-    <t>Zandy.yen@OneDigital.co</t>
-  </si>
-  <si>
-    <t>frank.leal@RobotInc.co</t>
+    <t>C:/Documents/Tita/</t>
+  </si>
+  <si>
+    <t>C:/Documents/Tita/Docs/</t>
+  </si>
+  <si>
+    <t>rafael@2nv.co</t>
+  </si>
+  <si>
+    <t>jm@2nv.co</t>
+  </si>
+  <si>
+    <t>saul@2nv.co</t>
   </si>
 </sst>
 </file>
@@ -611,7 +608,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,18 +631,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,15 +658,15 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -677,15 +674,18 @@
         <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -693,15 +693,21 @@
         <v>5</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,193 +715,191 @@
         <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" display="camilotobon21@gmail.com" xr:uid="{15843C65-BEF1-4C7A-A697-B2A4FC778FEB}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{22498C91-5A82-4D20-987C-8FA72F7178DB}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{8AE32C83-F27F-4D09-BB8B-F5A586D37676}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>